<commit_message>
Feat: Include dockerfile and configure project
</commit_message>
<xml_diff>
--- a/games-compact.xlsx
+++ b/games-compact.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="games" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="36">
   <si>
     <t xml:space="preserve">Game Name</t>
   </si>
@@ -90,6 +90,45 @@
   </si>
   <si>
     <t xml:space="preserve">01/01/1982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unknown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selchow &amp; Righter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.vgchartz.com/games/boxart/1137241ccc.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/01/1983</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phaser Patrol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arcadia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.vgchartz.com/games/boxart/5877491ccc.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kool-Aid Man</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mattel Interactive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mattel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.vgchartz.com/games/boxart/775863ccc.jpg</t>
   </si>
 </sst>
 </file>
@@ -191,13 +230,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="92.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.99"/>
@@ -299,6 +338,75 @@
       </c>
       <c r="G4" s="1" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -317,13 +425,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="92.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.99"/>
@@ -427,6 +535,75 @@
         <v>22</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>